<commit_message>
research assignment notes, presentation, video link, and gantt chart
</commit_message>
<xml_diff>
--- a/hw6/project_plan.xlsx
+++ b/hw6/project_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11102"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monoble/Desktop/Database/CSCI331_group6/hw6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752AF14B-D4BB-A243-985F-37521C9780CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2972FA2C-8EFA-684F-9D0C-067F9BA50D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -145,43 +145,22 @@
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
   <si>
-    <t>Project Planning</t>
-  </si>
-  <si>
-    <t>Functional Specification</t>
-  </si>
-  <si>
-    <t>Assigning Propositions</t>
-  </si>
-  <si>
-    <t>Solve Propositions</t>
-  </si>
-  <si>
     <t>Group Discussion</t>
-  </si>
-  <si>
-    <t>Video Explanation</t>
-  </si>
-  <si>
-    <t>Push to GitHub Repo</t>
-  </si>
-  <si>
-    <t>Final Submission</t>
   </si>
   <si>
     <t>Day</t>
   </si>
   <si>
-    <t>Formulating Mysteries</t>
+    <t>Research Assignment Planner</t>
   </si>
   <si>
-    <t>Catchup with all chapters</t>
+    <t>Conduct Indivisual Research</t>
   </si>
   <si>
-    <t>Create NACE Presentation</t>
+    <t>Formulating Slides</t>
   </si>
   <si>
-    <t>Project 1 Planner</t>
+    <t>Film &amp; Edit Video Explanation</t>
   </si>
 </sst>
 </file>
@@ -987,10 +966,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO114"/>
+  <dimension ref="B1:BO107"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1004,7 +983,7 @@
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="12" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -1090,7 +1069,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="9"/>
@@ -1302,19 +1281,19 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C5" s="6">
         <v>1</v>
       </c>
       <c r="D5" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6">
         <v>1</v>
       </c>
       <c r="F5" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -1325,13 +1304,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
@@ -1342,16 +1321,16 @@
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
@@ -1362,16 +1341,16 @@
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
@@ -1381,144 +1360,200 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1</v>
-      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6">
-        <v>5</v>
-      </c>
-      <c r="F10" s="6">
-        <v>2</v>
-      </c>
-      <c r="G10" s="7">
-        <v>1</v>
-      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="6">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
-        <v>7</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <v>1</v>
-      </c>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="6">
-        <v>7</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6">
-        <v>7</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="6">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>8</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="6">
-        <v>8</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6">
-        <v>8</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="6">
-        <v>8</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <v>8</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1</v>
-      </c>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16"/>
@@ -4096,202 +4131,6 @@
       <c r="Z107"/>
       <c r="AA107"/>
     </row>
-    <row r="108" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108"/>
-      <c r="C108"/>
-      <c r="D108"/>
-      <c r="E108"/>
-      <c r="F108"/>
-      <c r="G108"/>
-      <c r="H108"/>
-      <c r="I108"/>
-      <c r="J108"/>
-      <c r="K108"/>
-      <c r="L108"/>
-      <c r="M108"/>
-      <c r="N108"/>
-      <c r="O108"/>
-      <c r="P108"/>
-      <c r="Q108"/>
-      <c r="R108"/>
-      <c r="S108"/>
-      <c r="T108"/>
-      <c r="U108"/>
-      <c r="V108"/>
-      <c r="W108"/>
-      <c r="X108"/>
-      <c r="Y108"/>
-      <c r="Z108"/>
-      <c r="AA108"/>
-    </row>
-    <row r="109" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109"/>
-      <c r="F109"/>
-      <c r="G109"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-      <c r="N109"/>
-      <c r="O109"/>
-      <c r="P109"/>
-      <c r="Q109"/>
-      <c r="R109"/>
-      <c r="S109"/>
-      <c r="T109"/>
-      <c r="U109"/>
-      <c r="V109"/>
-      <c r="W109"/>
-      <c r="X109"/>
-      <c r="Y109"/>
-      <c r="Z109"/>
-      <c r="AA109"/>
-    </row>
-    <row r="110" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B110"/>
-      <c r="C110"/>
-      <c r="D110"/>
-      <c r="E110"/>
-      <c r="F110"/>
-      <c r="G110"/>
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="J110"/>
-      <c r="K110"/>
-      <c r="L110"/>
-      <c r="M110"/>
-      <c r="N110"/>
-      <c r="O110"/>
-      <c r="P110"/>
-      <c r="Q110"/>
-      <c r="R110"/>
-      <c r="S110"/>
-      <c r="T110"/>
-      <c r="U110"/>
-      <c r="V110"/>
-      <c r="W110"/>
-      <c r="X110"/>
-      <c r="Y110"/>
-      <c r="Z110"/>
-      <c r="AA110"/>
-    </row>
-    <row r="111" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111"/>
-      <c r="C111"/>
-      <c r="D111"/>
-      <c r="E111"/>
-      <c r="F111"/>
-      <c r="G111"/>
-      <c r="H111"/>
-      <c r="I111"/>
-      <c r="J111"/>
-      <c r="K111"/>
-      <c r="L111"/>
-      <c r="M111"/>
-      <c r="N111"/>
-      <c r="O111"/>
-      <c r="P111"/>
-      <c r="Q111"/>
-      <c r="R111"/>
-      <c r="S111"/>
-      <c r="T111"/>
-      <c r="U111"/>
-      <c r="V111"/>
-      <c r="W111"/>
-      <c r="X111"/>
-      <c r="Y111"/>
-      <c r="Z111"/>
-      <c r="AA111"/>
-    </row>
-    <row r="112" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B112"/>
-      <c r="C112"/>
-      <c r="D112"/>
-      <c r="E112"/>
-      <c r="F112"/>
-      <c r="G112"/>
-      <c r="H112"/>
-      <c r="I112"/>
-      <c r="J112"/>
-      <c r="K112"/>
-      <c r="L112"/>
-      <c r="M112"/>
-      <c r="N112"/>
-      <c r="O112"/>
-      <c r="P112"/>
-      <c r="Q112"/>
-      <c r="R112"/>
-      <c r="S112"/>
-      <c r="T112"/>
-      <c r="U112"/>
-      <c r="V112"/>
-      <c r="W112"/>
-      <c r="X112"/>
-      <c r="Y112"/>
-      <c r="Z112"/>
-      <c r="AA112"/>
-    </row>
-    <row r="113" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113"/>
-      <c r="C113"/>
-      <c r="D113"/>
-      <c r="E113"/>
-      <c r="F113"/>
-      <c r="G113"/>
-      <c r="H113"/>
-      <c r="I113"/>
-      <c r="J113"/>
-      <c r="K113"/>
-      <c r="L113"/>
-      <c r="M113"/>
-      <c r="N113"/>
-      <c r="O113"/>
-      <c r="P113"/>
-      <c r="Q113"/>
-      <c r="R113"/>
-      <c r="S113"/>
-      <c r="T113"/>
-      <c r="U113"/>
-      <c r="V113"/>
-      <c r="W113"/>
-      <c r="X113"/>
-      <c r="Y113"/>
-      <c r="Z113"/>
-      <c r="AA113"/>
-    </row>
-    <row r="114" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B114"/>
-      <c r="C114"/>
-      <c r="D114"/>
-      <c r="E114"/>
-      <c r="F114"/>
-      <c r="G114"/>
-      <c r="H114"/>
-      <c r="I114"/>
-      <c r="J114"/>
-      <c r="K114"/>
-      <c r="L114"/>
-      <c r="M114"/>
-      <c r="N114"/>
-      <c r="O114"/>
-      <c r="P114"/>
-      <c r="Q114"/>
-      <c r="R114"/>
-      <c r="S114"/>
-      <c r="T114"/>
-      <c r="U114"/>
-      <c r="V114"/>
-      <c r="W114"/>
-      <c r="X114"/>
-      <c r="Y114"/>
-      <c r="Z114"/>
-      <c r="AA114"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="AI2:AP2"/>
@@ -4313,7 +4152,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO15">
+  <conditionalFormatting sqref="H5:BO8">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>